<commit_message>
More QTI Picks #4s
</commit_message>
<xml_diff>
--- a/static/documents/qti_portfolio.xlsx
+++ b/static/documents/qti_portfolio.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Agasthya\Desktop\ASP\static\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F0A3ED5-A939-4E11-B49C-60334DCF56F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2252C710-585C-41AD-BD1F-E22EEE689E0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
   <si>
     <t>Company Name</t>
   </si>
@@ -89,15 +89,6 @@
     <t>BA</t>
   </si>
   <si>
-    <t>Buy</t>
-  </si>
-  <si>
-    <t>GE Aerospace Inc.</t>
-  </si>
-  <si>
-    <t>GE</t>
-  </si>
-  <si>
     <t>10/21/24</t>
   </si>
   <si>
@@ -105,6 +96,21 @@
   </si>
   <si>
     <t>NKE</t>
+  </si>
+  <si>
+    <t>Pfizer Inc.</t>
+  </si>
+  <si>
+    <t>PFE</t>
+  </si>
+  <si>
+    <t>10/18/24</t>
+  </si>
+  <si>
+    <t>AMD</t>
+  </si>
+  <si>
+    <t>10/10/24</t>
   </si>
 </sst>
 </file>
@@ -494,10 +500,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -599,22 +605,22 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D5" s="4">
-        <v>193.68</v>
+        <v>165.35</v>
       </c>
       <c r="F5" s="4">
-        <v>187</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>21</v>
+        <v>0</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -622,10 +628,10 @@
         <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D6" s="4">
         <v>82.61</v>
@@ -634,7 +640,27 @@
         <v>0</v>
       </c>
       <c r="H6" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
         <v>21</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="4">
+        <v>29.17</v>
+      </c>
+      <c r="F7" s="4">
+        <v>0</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>